<commit_message>
Daily Status xl sheet updated
</commit_message>
<xml_diff>
--- a/documents/Daily Status.xlsx
+++ b/documents/Daily Status.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7965" tabRatio="815" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7965" tabRatio="815" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Training Student Name" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="507">
   <si>
     <t xml:space="preserve">Name Of Student </t>
   </si>
@@ -3860,7 +3860,58 @@
     <t>8th Feb</t>
   </si>
   <si>
-    <t>dd</t>
+    <t>10th feb</t>
+  </si>
+  <si>
+    <t>Given to sachin</t>
+  </si>
+  <si>
+    <t>3rd Feb</t>
+  </si>
+  <si>
+    <t>1500 Paid 11th Feb</t>
+  </si>
+  <si>
+    <t>Pushpendra Singh</t>
+  </si>
+  <si>
+    <t>pushp.singh94@gmail.com</t>
+  </si>
+  <si>
+    <t>I.I.M.T</t>
+  </si>
+  <si>
+    <t>Quadcopter</t>
+  </si>
+  <si>
+    <t>Umesh</t>
+  </si>
+  <si>
+    <t>umeshnamdev9@gmail.com</t>
+  </si>
+  <si>
+    <t>11th Feb</t>
+  </si>
+  <si>
+    <t>Card Board</t>
+  </si>
+  <si>
+    <t>Card Board Cutting</t>
+  </si>
+  <si>
+    <t>PVC Tape</t>
+  </si>
+  <si>
+    <t>Tape</t>
+  </si>
+  <si>
+    <t>Navneet</t>
+  </si>
+  <si>
+    <t>navneetsharme1996@rediffmail.co.in</t>
+  </si>
+  <si>
+    <t>11Th Feb</t>
   </si>
 </sst>
 </file>
@@ -3932,7 +3983,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3990,6 +4041,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4083,7 +4140,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -4259,6 +4316,23 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="11" borderId="3" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="11" borderId="3" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="4" xfId="2" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4565,7 +4639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -4691,8 +4765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5148,8 +5222,8 @@
       <c r="D18" t="s">
         <v>437</v>
       </c>
-      <c r="E18" s="80">
-        <v>42038</v>
+      <c r="E18" s="80" t="s">
+        <v>491</v>
       </c>
       <c r="F18">
         <v>20</v>
@@ -5176,8 +5250,26 @@
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="B20" t="s">
-        <v>489</v>
+      <c r="A20" t="s">
+        <v>504</v>
+      </c>
+      <c r="B20">
+        <v>8375940733</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>505</v>
+      </c>
+      <c r="D20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" t="s">
+        <v>506</v>
+      </c>
+      <c r="F20">
+        <v>400</v>
+      </c>
+      <c r="H20" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -5195,18 +5287,19 @@
     <hyperlink ref="C15" r:id="rId11"/>
     <hyperlink ref="C16" r:id="rId12"/>
     <hyperlink ref="C17" r:id="rId13"/>
+    <hyperlink ref="C20" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId14"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId15"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5466,6 +5559,40 @@
         <v>486</v>
       </c>
     </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>493</v>
+      </c>
+      <c r="B14">
+        <v>9990036755</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>494</v>
+      </c>
+      <c r="D14" t="s">
+        <v>495</v>
+      </c>
+      <c r="E14" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>497</v>
+      </c>
+      <c r="B15">
+        <v>9540424976</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="D15" t="s">
+        <v>495</v>
+      </c>
+      <c r="E15" t="s">
+        <v>496</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
@@ -5480,6 +5607,8 @@
     <hyperlink ref="C11" r:id="rId10"/>
     <hyperlink ref="C12" r:id="rId11"/>
     <hyperlink ref="C13" r:id="rId12"/>
+    <hyperlink ref="C14" r:id="rId13"/>
+    <hyperlink ref="C15" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5514,10 +5643,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5725,6 +5854,61 @@
       </c>
       <c r="C18">
         <v>500</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>489</v>
+      </c>
+      <c r="B19" t="s">
+        <v>490</v>
+      </c>
+      <c r="C19">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>489</v>
+      </c>
+      <c r="B20" t="s">
+        <v>451</v>
+      </c>
+      <c r="C20">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>499</v>
+      </c>
+      <c r="B21" t="s">
+        <v>500</v>
+      </c>
+      <c r="C21">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>499</v>
+      </c>
+      <c r="B22" t="s">
+        <v>501</v>
+      </c>
+      <c r="C22">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>502</v>
+      </c>
+      <c r="B23" t="s">
+        <v>503</v>
+      </c>
+      <c r="C23">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -5970,9 +6154,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -5988,7 +6172,7 @@
     <col min="9" max="9" width="14.85546875" style="11" customWidth="1"/>
     <col min="10" max="10" width="16.140625" style="11" customWidth="1"/>
     <col min="11" max="11" width="26.42578125" style="13" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="14"/>
+    <col min="12" max="12" width="24.28515625" style="14" customWidth="1"/>
     <col min="13" max="257" width="9.140625" style="15"/>
     <col min="258" max="258" width="27.7109375" style="15" customWidth="1"/>
     <col min="259" max="259" width="15.28515625" style="15" customWidth="1"/>
@@ -6722,35 +6906,35 @@
       <c r="L1" s="9"/>
     </row>
     <row r="2" spans="1:12" ht="13.5" thickBot="1"/>
-    <row r="3" spans="1:12" s="22" customFormat="1" ht="26.25" thickBot="1">
-      <c r="A3" s="16">
+    <row r="3" spans="1:12" s="87" customFormat="1" ht="13.5" thickBot="1">
+      <c r="A3" s="81">
         <v>1</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="82" t="s">
         <v>98</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C3" s="83">
         <v>41907</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="84" t="s">
         <v>99</v>
       </c>
-      <c r="E3" s="20"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17">
+      <c r="E3" s="85"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82">
         <v>9555382729</v>
       </c>
-      <c r="H3" s="16">
+      <c r="H3" s="81">
         <v>6000</v>
       </c>
-      <c r="I3" s="16">
+      <c r="I3" s="81">
         <v>100</v>
       </c>
-      <c r="J3" s="16"/>
-      <c r="K3" s="20" t="s">
-        <v>353</v>
-      </c>
-      <c r="L3" s="21"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="85" t="s">
+        <v>492</v>
+      </c>
+      <c r="L3" s="86"/>
     </row>
     <row r="4" spans="1:12" s="71" customFormat="1" ht="26.25" thickBot="1">
       <c r="A4" s="64">

</xml_diff>

<commit_message>
daily status sheet has been updated
</commit_message>
<xml_diff>
--- a/documents/Daily Status.xlsx
+++ b/documents/Daily Status.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7965" tabRatio="815" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7965" tabRatio="815" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Training Student Name" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="515">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="519">
   <si>
     <t xml:space="preserve">Name Of Student </t>
   </si>
@@ -3936,6 +3936,18 @@
   </si>
   <si>
     <t>Actual Balance in Lab</t>
+  </si>
+  <si>
+    <t>Ayushi Gupta</t>
+  </si>
+  <si>
+    <t>ayushigauri18@gmail.com</t>
+  </si>
+  <si>
+    <t>G.U</t>
+  </si>
+  <si>
+    <t>Tabbaco Tracking Asp.net</t>
   </si>
 </sst>
 </file>
@@ -5320,10 +5332,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5615,6 +5627,23 @@
       </c>
       <c r="E15" t="s">
         <v>495</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>515</v>
+      </c>
+      <c r="B16">
+        <v>7042248420</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>516</v>
+      </c>
+      <c r="D16" t="s">
+        <v>517</v>
+      </c>
+      <c r="E16" t="s">
+        <v>518</v>
       </c>
     </row>
   </sheetData>
@@ -5633,6 +5662,7 @@
     <hyperlink ref="C13" r:id="rId12"/>
     <hyperlink ref="C14" r:id="rId13"/>
     <hyperlink ref="C15" r:id="rId14"/>
+    <hyperlink ref="C16" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5642,7 +5672,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>